<commit_message>
chagement de taille des images / bloc 1 3 modif contrast
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jukem\Desktop\Projet4\JulienKemena_4_29072021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E0043B-C70F-4E20-954C-0DBDBC345323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DEA4F4-9C44-4BAD-AB0E-9BB1517F6E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
correction au w3c et changement du bouton contact
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jukem\Desktop\Projet4\JulienKemena_4_29072021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DEA4F4-9C44-4BAD-AB0E-9BB1517F6E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC97F5F3-5182-44FD-8190-055F006BC0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>Catégorie</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Réduire a une taille adapté avec un site adapté pour changer une taille d'image</t>
+  </si>
+  <si>
+    <t>erreur 404</t>
+  </si>
+  <si>
+    <t>aria</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -808,9 +814,21 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
modif du fichier excel
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jukem\Desktop\Projet4\JulienKemena_4_29072021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F45362A-A904-48C0-BC7A-575B7501554D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62C25B7-A26C-4421-8FC6-C8817CD38C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>Catégorie</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>h1 plus pertinent</t>
+  </si>
+  <si>
+    <t>https://www.zeemedia.fr/metiers/titre-h1-seo/</t>
   </si>
 </sst>
 </file>
@@ -562,7 +565,7 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -829,6 +832,9 @@
       </c>
       <c r="E13" s="6" t="s">
         <v>43</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1861,8 +1867,9 @@
     <hyperlink ref="F12" r:id="rId6" xr:uid="{4406EC48-3573-4650-9EDF-054E5C843C3D}"/>
     <hyperlink ref="F6" r:id="rId7" xr:uid="{F19075E7-99B7-41EA-9937-95E37226CC7D}"/>
     <hyperlink ref="F14" r:id="rId8" xr:uid="{43274F5F-DACF-4545-9F1C-19B67689DA3B}"/>
+    <hyperlink ref="F13" r:id="rId9" xr:uid="{D2818136-FBF9-4D1C-BF9F-2BD84DA2A8C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId9"/>
+  <pageSetup orientation="landscape" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modif alt text des images bloc 4
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jukem\Desktop\Projet4\JulienKemena_4_29072021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62C25B7-A26C-4421-8FC6-C8817CD38C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814D30CD-38DC-4656-8F29-798E10EF1362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,9 +114,6 @@
     <t xml:space="preserve">N’utilisez pas de liens ou de textes cachés pour aumgenter le réferencement </t>
   </si>
   <si>
-    <t>Supprimer toutes techmiques de Black-hat</t>
-  </si>
-  <si>
     <t xml:space="preserve">mettre une langue approprié au site </t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>Point 7 https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t>
   </si>
   <si>
-    <t>https://openweb.eu.org/articles/accessibilite_images (les images significatives)</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Element/title </t>
   </si>
   <si>
@@ -247,6 +241,12 @@
   </si>
   <si>
     <t>https://www.zeemedia.fr/metiers/titre-h1-seo/</t>
+  </si>
+  <si>
+    <t>https://openweb.eu.org/articles/accessibilite_images (les images significatives point 3)</t>
+  </si>
+  <si>
+    <t>Supprimer toutes techniques de Black-hat</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -636,7 +636,7 @@
         <v>24</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -650,13 +650,13 @@
         <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -673,10 +673,10 @@
         <v>25</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -684,19 +684,19 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -713,10 +713,10 @@
         <v>18</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -730,13 +730,13 @@
         <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="F8" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -744,19 +744,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
         <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -764,19 +764,19 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="F10" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -784,19 +784,19 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -804,17 +804,17 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -822,19 +822,19 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -842,17 +842,17 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -860,16 +860,16 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>